<commit_message>
docker container script can access arcgis successfully
</commit_message>
<xml_diff>
--- a/reverse_engineer_API/test_data/Aerial_Status_Tracker.xlsx
+++ b/reverse_engineer_API/test_data/Aerial_Status_Tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +511,7 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:54.768172</t>
+          <t>2025-01-02T19:48:12.732734</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:22.921808</t>
+          <t>2025-01-02T19:47:40.914400</t>
         </is>
       </c>
     </row>
@@ -581,7 +581,7 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:30.342022</t>
+          <t>2025-01-02T19:46:48.080180</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:27.631535</t>
+          <t>2025-01-02T19:46:45.374822</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:18.341925</t>
+          <t>2025-01-02T19:46:36.170178</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:01.663792</t>
+          <t>2025-01-02T19:47:19.789096</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:07.269313</t>
+          <t>2025-01-02T19:47:25.892795</t>
         </is>
       </c>
     </row>
@@ -756,7 +756,7 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:10.425584</t>
+          <t>2025-01-02T19:47:28.895664</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2025-01-02T19:35:56.440011</t>
+          <t>2025-01-02T19:46:15.052312</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2025-01-02T19:35:53.396196</t>
+          <t>2025-01-02T19:46:11.933472</t>
         </is>
       </c>
     </row>
@@ -861,7 +861,7 @@
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:09.554107</t>
+          <t>2025-01-02T19:46:27.469020</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:52.204386</t>
+          <t>2025-01-02T19:48:10.069169</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:30.366395</t>
+          <t>2025-01-02T19:48:47.984714</t>
         </is>
       </c>
     </row>
@@ -974,7 +974,7 @@
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:52.591240</t>
+          <t>2025-01-02T19:47:11.240757</t>
         </is>
       </c>
     </row>
@@ -1009,7 +1009,7 @@
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:55.038015</t>
+          <t>2025-01-02T19:47:13.739001</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:57.385631</t>
+          <t>2025-01-02T19:47:16.148224</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:08.318670</t>
+          <t>2025-01-02T19:49:26.181621</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:33.477845</t>
+          <t>2025-01-02T19:46:51.010762</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       <c r="H20" t="inlineStr"/>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:57.399671</t>
+          <t>2025-01-02T19:48:15.189939</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1196,7 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:19.709146</t>
+          <t>2025-01-02T19:47:37.897898</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:32.964938</t>
+          <t>2025-01-02T19:47:51.230079</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:30.479984</t>
+          <t>2025-01-02T19:47:48.770174</t>
         </is>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:07.621892</t>
+          <t>2025-01-02T19:48:25.383272</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
       <c r="H25" t="inlineStr"/>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:35.637505</t>
+          <t>2025-01-02T19:47:54.038739</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:38.153819</t>
+          <t>2025-01-02T19:47:56.599736</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:25.661963</t>
+          <t>2025-01-02T19:49:42.545930</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:41.341471</t>
+          <t>2025-01-02T19:47:59.207786</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:43.795159</t>
+          <t>2025-01-02T19:48:01.616058</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       <c r="H30" t="inlineStr"/>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:46.702413</t>
+          <t>2025-01-02T19:48:04.046918</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       <c r="H31" t="inlineStr"/>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:23.073070</t>
+          <t>2025-01-02T19:49:40.072531</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:50.221611</t>
+          <t>2025-01-02T19:49:08.291843</t>
         </is>
       </c>
     </row>
@@ -1620,7 +1620,7 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:52.863482</t>
+          <t>2025-01-02T19:49:10.665336</t>
         </is>
       </c>
     </row>
@@ -1655,7 +1655,7 @@
       <c r="H34" t="inlineStr"/>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:55.415976</t>
+          <t>2025-01-02T19:49:13.163910</t>
         </is>
       </c>
     </row>
@@ -1690,7 +1690,7 @@
       <c r="H35" t="inlineStr"/>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:57.819345</t>
+          <t>2025-01-02T19:49:15.564511</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       <c r="H36" t="inlineStr"/>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:00.501141</t>
+          <t>2025-01-02T19:49:18.350011</t>
         </is>
       </c>
     </row>
@@ -1760,7 +1760,7 @@
       <c r="H37" t="inlineStr"/>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:02.949366</t>
+          <t>2025-01-02T19:49:20.830268</t>
         </is>
       </c>
     </row>
@@ -1795,7 +1795,7 @@
       <c r="H38" t="inlineStr"/>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:05.501367</t>
+          <t>2025-01-02T19:49:23.350637</t>
         </is>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:59.810984</t>
+          <t>2025-01-02T19:48:17.781378</t>
         </is>
       </c>
     </row>
@@ -1865,7 +1865,7 @@
       <c r="H40" t="inlineStr"/>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:32.818274</t>
+          <t>2025-01-02T19:48:50.494249</t>
         </is>
       </c>
     </row>
@@ -1900,7 +1900,7 @@
       <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:35.318687</t>
+          <t>2025-01-02T19:48:52.855991</t>
         </is>
       </c>
     </row>
@@ -1935,7 +1935,7 @@
       <c r="H42" t="inlineStr"/>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:37.669813</t>
+          <t>2025-01-02T19:48:55.393064</t>
         </is>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:40.310277</t>
+          <t>2025-01-02T19:48:58.088132</t>
         </is>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
       <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:42.863062</t>
+          <t>2025-01-02T19:49:00.723760</t>
         </is>
       </c>
     </row>
@@ -2040,7 +2040,7 @@
       <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:45.253613</t>
+          <t>2025-01-02T19:49:03.272346</t>
         </is>
       </c>
     </row>
@@ -2075,7 +2075,7 @@
       <c r="H46" t="inlineStr"/>
       <c r="I46" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:47.729029</t>
+          <t>2025-01-02T19:49:05.710687</t>
         </is>
       </c>
     </row>
@@ -2110,7 +2110,7 @@
       <c r="H47" t="inlineStr"/>
       <c r="I47" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:02.331629</t>
+          <t>2025-01-02T19:48:20.198641</t>
         </is>
       </c>
     </row>
@@ -2145,7 +2145,7 @@
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:04.923009</t>
+          <t>2025-01-02T19:48:22.703004</t>
         </is>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:10.053720</t>
+          <t>2025-01-02T19:48:27.834087</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:12.890007</t>
+          <t>2025-01-02T19:48:30.432311</t>
         </is>
       </c>
     </row>
@@ -2250,7 +2250,7 @@
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:15.295501</t>
+          <t>2025-01-02T19:48:32.981408</t>
         </is>
       </c>
     </row>
@@ -2285,7 +2285,7 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:17.906574</t>
+          <t>2025-01-02T19:48:35.448585</t>
         </is>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:20.422542</t>
+          <t>2025-01-02T19:48:38.080283</t>
         </is>
       </c>
     </row>
@@ -2355,7 +2355,7 @@
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:26.352996</t>
+          <t>2025-01-02T19:48:43.658152</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:28.047507</t>
+          <t>2025-01-02T19:47:46.323832</t>
         </is>
       </c>
     </row>
@@ -2425,7 +2425,7 @@
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:49.155334</t>
+          <t>2025-01-02T19:47:07.416753</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2460,7 @@
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:17.566225</t>
+          <t>2025-01-02T19:49:34.717297</t>
         </is>
       </c>
     </row>
@@ -2495,7 +2495,7 @@
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:20.449780</t>
+          <t>2025-01-02T19:49:37.537657</t>
         </is>
       </c>
     </row>
@@ -2530,7 +2530,7 @@
       <c r="H59" t="inlineStr"/>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:14.327469</t>
+          <t>2025-01-02T19:49:31.712909</t>
         </is>
       </c>
     </row>
@@ -2565,7 +2565,7 @@
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:46.076341</t>
+          <t>2025-01-02T19:47:04.340938</t>
         </is>
       </c>
     </row>
@@ -2600,7 +2600,7 @@
       <c r="H61" t="inlineStr"/>
       <c r="I61" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:13.941300</t>
+          <t>2025-01-02T19:47:32.075484</t>
         </is>
       </c>
     </row>
@@ -2635,7 +2635,7 @@
       <c r="H62" t="inlineStr"/>
       <c r="I62" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:17.296841</t>
+          <t>2025-01-02T19:47:35.470642</t>
         </is>
       </c>
     </row>
@@ -2670,7 +2670,7 @@
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:39.262355</t>
+          <t>2025-01-02T19:46:57.267610</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>2025-01-02T19:38:23.558807</t>
+          <t>2025-01-02T19:48:41.192438</t>
         </is>
       </c>
     </row>
@@ -2748,7 +2748,7 @@
       <c r="H65" t="inlineStr"/>
       <c r="I65" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:36.048708</t>
+          <t>2025-01-02T19:46:53.635181</t>
         </is>
       </c>
     </row>
@@ -2783,7 +2783,7 @@
       <c r="H66" t="inlineStr"/>
       <c r="I66" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:41.853495</t>
+          <t>2025-01-02T19:46:59.842999</t>
         </is>
       </c>
     </row>
@@ -2818,7 +2818,7 @@
       <c r="H67" t="inlineStr"/>
       <c r="I67" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:12.517561</t>
+          <t>2025-01-02T19:46:30.511521</t>
         </is>
       </c>
     </row>
@@ -2853,7 +2853,7 @@
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:15.647244</t>
+          <t>2025-01-02T19:46:33.581522</t>
         </is>
       </c>
     </row>
@@ -2888,7 +2888,7 @@
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:20.866821</t>
+          <t>2025-01-02T19:46:38.704292</t>
         </is>
       </c>
     </row>
@@ -2923,7 +2923,7 @@
       <c r="H70" t="inlineStr"/>
       <c r="I70" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:49.302575</t>
+          <t>2025-01-02T19:48:07.006848</t>
         </is>
       </c>
     </row>
@@ -2958,7 +2958,7 @@
       <c r="H71" t="inlineStr"/>
       <c r="I71" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:25.478687</t>
+          <t>2025-01-02T19:47:43.629638</t>
         </is>
       </c>
     </row>
@@ -2993,7 +2993,7 @@
       <c r="H72" t="inlineStr"/>
       <c r="I72" t="inlineStr">
         <is>
-          <t>2025-01-02T19:37:04.395222</t>
+          <t>2025-01-02T19:47:22.445001</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       <c r="A73" t="inlineStr"/>
       <c r="B73" t="inlineStr">
         <is>
-          <t>VZN_Electra</t>
+          <t>Update_Test_New</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3022,13 +3022,17 @@
       <c r="F73" t="inlineStr"/>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr"/>
+          <t>Testing</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Used to test daily automated sync</t>
+        </is>
+      </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:06.487005</t>
+          <t>2025-01-02T19:49:44.918217</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3040,7 @@
       <c r="A74" t="inlineStr"/>
       <c r="B74" t="inlineStr">
         <is>
-          <t>VZN_FloridaMesa</t>
+          <t>VZN_Electra</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -3063,7 +3067,7 @@
       <c r="H74" t="inlineStr"/>
       <c r="I74" t="inlineStr">
         <is>
-          <t>2025-01-02T19:35:59.028583</t>
+          <t>2025-01-02T19:46:24.696098</t>
         </is>
       </c>
     </row>
@@ -3071,7 +3075,7 @@
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr">
         <is>
-          <t>VZN_Pagosa</t>
+          <t>VZN_FloridaMesa</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -3098,7 +3102,7 @@
       <c r="H75" t="inlineStr"/>
       <c r="I75" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:01.399485</t>
+          <t>2025-01-02T19:46:17.494802</t>
         </is>
       </c>
     </row>
@@ -3106,7 +3110,7 @@
       <c r="A76" t="inlineStr"/>
       <c r="B76" t="inlineStr">
         <is>
-          <t>VZN_Rifle</t>
+          <t>VZN_Pagosa</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -3133,7 +3137,7 @@
       <c r="H76" t="inlineStr"/>
       <c r="I76" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:03.943163</t>
+          <t>2025-01-02T19:46:19.891900</t>
         </is>
       </c>
     </row>
@@ -3141,7 +3145,7 @@
       <c r="A77" t="inlineStr"/>
       <c r="B77" t="inlineStr">
         <is>
-          <t>cortezmisc</t>
+          <t>VZN_Rifle</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3168,7 +3172,7 @@
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
         <is>
-          <t>2025-01-02T19:39:11.489580</t>
+          <t>2025-01-02T19:46:22.305474</t>
         </is>
       </c>
     </row>
@@ -3176,7 +3180,7 @@
       <c r="A78" t="inlineStr"/>
       <c r="B78" t="inlineStr">
         <is>
-          <t>fruita extras</t>
+          <t>cortezmisc</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3203,7 +3207,42 @@
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr">
         <is>
-          <t>2025-01-02T19:36:24.053773</t>
+          <t>2025-01-02T19:49:29.008045</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>fruita extras</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Unassigned</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2025-01-02T19:46:41.751123</t>
         </is>
       </c>
     </row>

</xml_diff>